<commit_message>
+ code refactor + gitkeep files
</commit_message>
<xml_diff>
--- a/xlsx/hosts.xlsx
+++ b/xlsx/hosts.xlsx
@@ -1,42 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\_scripts\_scripts\netops\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\_scripts\netops\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4113AB4-2E60-4A9E-8FE7-A9AE0B19910A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7CD8F2-5E42-4FE4-B389-B4CBA9449601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AA$2</definedName>
-  </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
-  <si>
-    <t>Cisco</t>
-  </si>
-  <si>
-    <t>WS-C4948</t>
-  </si>
-  <si>
-    <t>cisco_ios_telnet</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Exec</t>
   </si>
   <si>
+    <t>Location</t>
+  </si>
+  <si>
     <t>KVO</t>
   </si>
   <si>
@@ -112,41 +103,33 @@
     <t>X</t>
   </si>
   <si>
-    <t>1.1.1.1</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Location</t>
+    <t>1.1.1.190</t>
+  </si>
+  <si>
+    <t>1.1.1.195</t>
+  </si>
+  <si>
+    <t>cisco_ios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -185,18 +168,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -208,59 +190,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1588</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>1588</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2" descr="http://5B562383578B10940AA830D2A608F829.dms.sberbank.ru/5B562383578B10940AA830D2A608F829-FA5B056D6C5A56B445BFEE60CFE87FF0-3AC6363096276D27575C04848EB50529/1.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:link="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1588" cy="1588"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -298,9 +231,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -333,9 +266,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -368,9 +318,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -402,16 +369,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -533,182 +504,128 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="I2" sqref="I2:AC6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="20.8984375" customWidth="1"/>
-    <col min="6" max="6" width="20.3984375" customWidth="1"/>
-    <col min="7" max="7" width="8.59765625" customWidth="1"/>
-    <col min="8" max="10" width="20.8984375" customWidth="1"/>
-    <col min="11" max="11" width="27.09765625" customWidth="1"/>
-    <col min="12" max="12" width="20.8984375" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="F2" t="s">
         <v>27</v>
       </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="H3" t="s">
         <v>29</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="G2:H2 I2" numberStoredAsText="1"/>
-  </ignoredErrors>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+ send_config_ser verify:false fix
</commit_message>
<xml_diff>
--- a/xlsx/hosts.xlsx
+++ b/xlsx/hosts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\_scripts\netops\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7CD8F2-5E42-4FE4-B389-B4CBA9449601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0894E0-F1F7-4944-A0E0-F4ECCFEB14A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Exec</t>
   </si>
@@ -103,6 +103,12 @@
     <t>X</t>
   </si>
   <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
     <t>1.1.1.190</t>
   </si>
   <si>
@@ -110,6 +116,127 @@
   </si>
   <si>
     <t>cisco_ios</t>
+  </si>
+  <si>
+    <t>ssh</t>
+  </si>
+  <si>
+    <t>no errors</t>
+  </si>
+  <si>
+    <t>no error</t>
+  </si>
+  <si>
+    <t>vios_l2-adventerprisek9-m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cisco IOS Software, vios_l2 Software (vios_l2-ADVENTERPRISEK9-M), Version 15.2(CML_NIGHTLY_20190423)FLO_DSGS7, EARLY DEPLOYMENT DEVELOPMENT BUILD, synced to  V152_6_0_81_E
+Technical Support: http://www.cisco.com/techsupport
+Copyright (c) 1986-2019 by Cisco Systems, Inc.
+Compiled Tue 23-Apr-19 04:48 by mmen
+ROM: Bootstrap program is IOSv
+SW1 uptime is 6 hours, 41 minutes
+System returned to ROM by reload
+System image file is "flash0:/vios_l2-adventerprisek9-m"
+Last reload reason: Unknown reason
+This product contains cryptographic features and is subject to United
+States and local country laws governing import, export, transfer and
+use. Delivery of Cisco cryptographic products does not imply
+third-party authority to import, export, distribute or use encryption.
+Importers, exporters, distributors and users are responsible for
+compliance with U.S. and local country laws. By using this product you
+agree to comply with applicable laws and regulations. If you are unable
+to comply with U.S. and local laws, return this product immediately.
+A summary of U.S. laws governing Cisco cryptographic products may be found at:
+http://www.cisco.com/wwl/export/crypto/tool/stqrg.html
+If you require further assistance please contact us by sending email to
+export@cisco.com.
+Cisco IOSv () processor (revision 1.0) with 935161K/111616K bytes of memory.
+Processor board ID 9BQHFDLPE7P
+1 Virtual Ethernet interface
+8 Gigabit Ethernet interfaces
+DRAM configuration is 72 bits wide with parity disabled.
+256K bytes of non-volatile configuration memory.
+2097152K bytes of ATA System CompactFlash 0 (Read/Write)
+0K bytes of ATA CompactFlash 1 (Read/Write)
+0K bytes of ATA CompactFlash 2 (Read/Write)
+0K bytes of ATA CompactFlash 3 (Read/Write)
+Configuration register is 0x101
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cisco IOS Software, vios_l2 Software (vios_l2-ADVENTERPRISEK9-M), Version 15.2(CML_NIGHTLY_20190423)FLO_DSGS7, EARLY DEPLOYMENT DEVELOPMENT BUILD, synced to  V152_6_0_81_E
+Technical Support: http://www.cisco.com/techsupport
+Copyright (c) 1986-2019 by Cisco Systems, Inc.
+Compiled Tue 23-Apr-19 04:48 by mmen
+ROM: Bootstrap program is IOSv
+SW2 uptime is 6 hours, 25 minutes
+System returned to ROM by reload
+System image file is "flash0:/vios_l2-adventerprisek9-m"
+Last reload reason: Unknown reason
+This product contains cryptographic features and is subject to United
+States and local country laws governing import, export, transfer and
+use. Delivery of Cisco cryptographic products does not imply
+third-party authority to import, export, distribute or use encryption.
+Importers, exporters, distributors and users are responsible for
+compliance with U.S. and local country laws. By using this product you
+agree to comply with applicable laws and regulations. If you are unable
+to comply with U.S. and local laws, return this product immediately.
+A summary of U.S. laws governing Cisco cryptographic products may be found at:
+http://www.cisco.com/wwl/export/crypto/tool/stqrg.html
+If you require further assistance please contact us by sending email to
+export@cisco.com.
+Cisco IOSv () processor (revision 1.0) with 935161K/111616K bytes of memory.
+Processor board ID 9HR276JJI1R
+1 Virtual Ethernet interface
+8 Gigabit Ethernet interfaces
+DRAM configuration is 72 bits wide with parity disabled.
+256K bytes of non-volatile configuration memory.
+2097152K bytes of ATA System CompactFlash 0 (Read/Write)
+0K bytes of ATA CompactFlash 1 (Read/Write)
+0K bytes of ATA CompactFlash 2 (Read/Write)
+0K bytes of ATA CompactFlash 3 (Read/Write)
+Configuration register is 0x101
+</t>
+  </si>
+  <si>
+    <t>Capability Codes: R - Router, T - Trans Bridge, B - Source Route Bridge
+                  S - Switch, H - Host, I - IGMP, r - Repeater, P - Phone, 
+                  D - Remote, C - CVTA, M - Two-port Mac Relay 
+Device ID        Local Intrfce     Holdtme    Capability  Platform  Port ID
+MikroTik         Gig 0/1           100               R    MikroTik  LAN/ether2
+SW2.home.net     Gig 0/1           143             R S I            Gig 0/1
+Total cdp entries displayed : 2</t>
+  </si>
+  <si>
+    <t>Capability Codes: R - Router, T - Trans Bridge, B - Source Route Bridge
+                  S - Switch, H - Host, I - IGMP, r - Repeater, P - Phone, 
+                  D - Remote, C - CVTA, M - Two-port Mac Relay 
+Device ID        Local Intrfce     Holdtme    Capability  Platform  Port ID
+MikroTik         Gig 0/1           100               R    MikroTik  LAN/ether2
+SW1.home.net     Gig 0/1           125             R S I            Gig 0/1
+Total cdp entries displayed : 2</t>
+  </si>
+  <si>
+    <t>% LLDP is not enabled</t>
+  </si>
+  <si>
+    <t>Interface                      Status         Protocol Description
+Gi0/0                          up             up       TEST2022
+Gi0/1                          up             up       TEST2022
+Gi0/2                          up             up       TEST2022
+Gi0/3                          up             up       TEST2022
+Gi1/0                          up             up       TEST2022
+Gi1/1                          up             up       TEST2022
+Gi1/2                          up             up       TEST2022
+Gi1/3                          up             up       TEST2022
+Vl10                           up             up       TEST2022</t>
+  </si>
+  <si>
+    <t>interface_cmd.template</t>
+  </si>
+  <si>
+    <t>hosts_if.xlsx</t>
   </si>
 </sst>
 </file>
@@ -514,7 +641,7 @@
   <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:AC6"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,22 +734,88 @@
       <c r="A2" t="s">
         <v>26</v>
       </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>